<commit_message>
Updated RMA detail report
</commit_message>
<xml_diff>
--- a/Code/Failure_rate/November_2020.xlsx
+++ b/Code/Failure_rate/November_2020.xlsx
@@ -6766,7 +6766,7 @@
         <v>32</v>
       </c>
       <c t="s" r="O49" s="1">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="P49" s="1">
         <v>0</v>
@@ -6840,7 +6840,7 @@
         <v>32</v>
       </c>
       <c t="s" r="O50" s="1">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="P50" s="1">
         <v>0</v>
@@ -6914,7 +6914,7 @@
         <v>32</v>
       </c>
       <c t="s" r="O51" s="1">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="P51" s="1">
         <v>0</v>

</xml_diff>